<commit_message>
BNC footprint is made manually
</commit_message>
<xml_diff>
--- a/Component/Component.xlsx
+++ b/Component/Component.xlsx
@@ -1,42 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jeonghyun\GIT\PMOD2BNC\Component\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\PMOD2BNC\Component\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40723E7-D80D-4DE8-82B3-0B377A1C0497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A261C83-5AE9-4556-88A0-7BD0218AEE66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15400" xr2:uid="{C77A721F-6D4C-4093-9F94-2F280AC7B0D4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12795" windowHeight="15405" activeTab="1" xr2:uid="{C77A721F-6D4C-4093-9F94-2F280AC7B0D4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="W Isolator" sheetId="1" r:id="rId1"/>
+    <sheet name="WO Isolator" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
   <si>
     <t>LD29150DT33R</t>
   </si>
@@ -303,6 +293,19 @@
   <si>
     <t>MAASL063SB7103MFCA01</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CONBC001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.mouser.kr/ProductDetail/TE-Connectivity-Linx-Technologies/CONBNC001?qs=doiCPypUmgHczHAGaJs8Lg%3D%3D</t>
+  </si>
+  <si>
+    <t>MULTICOMP PRO - MP-13-22-1</t>
+  </si>
+  <si>
+    <t>https://www.devicemart.co.kr/goods/view?no=12018713</t>
   </si>
 </sst>
 </file>
@@ -689,15 +692,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE501F11-C088-4299-BF8B-03B39C2617FD}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="25.08203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.4140625" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="25.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="34.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1082,6 +1085,193 @@
       <c r="D29" t="s">
         <v>73</v>
       </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D885F538-8857-439E-A6A7-C374B441810A}">
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="25.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="34.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
schematic and layout done. Delay is matched to 0.689ns. Making ground plane, and setting thickness of PCB is left
</commit_message>
<xml_diff>
--- a/Component/Component.xlsx
+++ b/Component/Component.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\PMOD2BNC\Component\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A261C83-5AE9-4556-88A0-7BD0218AEE66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F593171E-67B4-42D5-97F6-5ADCF3B5174D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12795" windowHeight="15405" activeTab="1" xr2:uid="{C77A721F-6D4C-4093-9F94-2F280AC7B0D4}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="86">
   <si>
     <t>LD29150DT33R</t>
   </si>
@@ -306,6 +306,21 @@
   </si>
   <si>
     <t>https://www.devicemart.co.kr/goods/view?no=12018713</t>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pin Header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.devicemart.co.kr/goods/view?no=5810</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1113,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1230,12 +1245,23 @@
       <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
       <c r="D10" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="B11" s="1"/>
+      <c r="A11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" s="1"/>

</xml_diff>